<commit_message>
play with config file
</commit_message>
<xml_diff>
--- a/R/practice/configure shiny ui/bbos_user_config.xlsx
+++ b/R/practice/configure shiny ui/bbos_user_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catherine\Documents\Development\learning\R\practice\configure shiny ui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4691D2B-4204-45BD-B00F-8203EB494162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D1B83-95BC-4D9C-BAF1-11FC49171777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AAD3DC31-2CEF-44B9-956F-90112AADF1F0}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,7 +493,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1.01</v>

</xml_diff>